<commit_message>
11/30/2015 add new object in member account
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20730" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
-    <t>Test Case Name</t>
-  </si>
-  <si>
     <t>User Name</t>
   </si>
   <si>
@@ -30,9 +27,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>TS 1.1</t>
-  </si>
-  <si>
     <t>jakther@centerlight.org.qual</t>
   </si>
   <si>
@@ -63,7 +57,13 @@
     <t>Expected SandBox</t>
   </si>
   <si>
-    <t>Actuel SAndBox</t>
+    <t>Test_Name</t>
+  </si>
+  <si>
+    <t>1.TC.1.1</t>
+  </si>
+  <si>
+    <t>Actuel Result</t>
   </si>
 </sst>
 </file>
@@ -413,53 +413,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="F2" t="str">
         <f>IF(EXACT(D2,E2),"Pass","Fail")</f>
@@ -468,13 +473,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F5" si="0">IF(EXACT(D3,E3),"Pass","Fail")</f>
@@ -483,13 +491,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -498,44 +509,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>Fail</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <f>IF(,D2,E2)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" t="str">
-        <f>IF(D2=E2,"Pass","Fail")</f>
-        <v>Fail</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" t="str">
-        <f t="shared" ref="F11:F13" si="1">IF(D3=E3,"Pass","Fail")</f>
-        <v>Fail</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="str">
-        <f t="shared" si="1"/>
-        <v>Fail</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" t="str">
-        <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Update on 12/18/2015 10:10 am
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20730" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20730" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="204">
   <si>
     <t>User Name</t>
   </si>
@@ -64,6 +64,570 @@
   </si>
   <si>
     <t>Actuel Result</t>
+  </si>
+  <si>
+    <t>Abkhazian</t>
+  </si>
+  <si>
+    <t>Afar</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>Akan</t>
+  </si>
+  <si>
+    <t>Albanian</t>
+  </si>
+  <si>
+    <t>Amharic</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>Aragonese</t>
+  </si>
+  <si>
+    <t>Armenian</t>
+  </si>
+  <si>
+    <t>Assamese</t>
+  </si>
+  <si>
+    <t>Avaric</t>
+  </si>
+  <si>
+    <t>Avestan</t>
+  </si>
+  <si>
+    <t>Aymara</t>
+  </si>
+  <si>
+    <t>Azerbaijani</t>
+  </si>
+  <si>
+    <t>Bambara</t>
+  </si>
+  <si>
+    <t>Bashkir</t>
+  </si>
+  <si>
+    <t>Basque</t>
+  </si>
+  <si>
+    <t>Bassa</t>
+  </si>
+  <si>
+    <t>Belarusian</t>
+  </si>
+  <si>
+    <t>Bengali</t>
+  </si>
+  <si>
+    <t>Bihari languages</t>
+  </si>
+  <si>
+    <t>Bislama</t>
+  </si>
+  <si>
+    <t>Bosnian</t>
+  </si>
+  <si>
+    <t>Breton</t>
+  </si>
+  <si>
+    <t>Bulgarian</t>
+  </si>
+  <si>
+    <t>Burmese</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>Central Khmer</t>
+  </si>
+  <si>
+    <t>Chamorro</t>
+  </si>
+  <si>
+    <t>Chechen</t>
+  </si>
+  <si>
+    <t>Chichewa</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Church Slavic</t>
+  </si>
+  <si>
+    <t>Chuvash</t>
+  </si>
+  <si>
+    <t>Cornish</t>
+  </si>
+  <si>
+    <t>Corsican</t>
+  </si>
+  <si>
+    <t>Cree</t>
+  </si>
+  <si>
+    <t>Croatian</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Declined to Specify or Unknown</t>
+  </si>
+  <si>
+    <t>Divehi</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>Dzongkha</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Esperanto</t>
+  </si>
+  <si>
+    <t>Estonian</t>
+  </si>
+  <si>
+    <t>Ewe</t>
+  </si>
+  <si>
+    <t>Faroese</t>
+  </si>
+  <si>
+    <t>Fijian</t>
+  </si>
+  <si>
+    <t>Fillipino</t>
+  </si>
+  <si>
+    <t>Finnish</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>French Creole</t>
+  </si>
+  <si>
+    <t>Fulah</t>
+  </si>
+  <si>
+    <t>Galician</t>
+  </si>
+  <si>
+    <t>Ganda</t>
+  </si>
+  <si>
+    <t>Georgian</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Greenlandic</t>
+  </si>
+  <si>
+    <t>Guarani</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>Haitian</t>
+  </si>
+  <si>
+    <t>Hausa</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>Herero</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Hiri Motu</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Icelandic</t>
+  </si>
+  <si>
+    <t>Ido</t>
+  </si>
+  <si>
+    <t>Igbo</t>
+  </si>
+  <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>Interlingua</t>
+  </si>
+  <si>
+    <t>Interlingue</t>
+  </si>
+  <si>
+    <t>Inuktitut</t>
+  </si>
+  <si>
+    <t>Inupiaq</t>
+  </si>
+  <si>
+    <t>Irish</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Kannada</t>
+  </si>
+  <si>
+    <t>Kanuri</t>
+  </si>
+  <si>
+    <t>Kashmiri</t>
+  </si>
+  <si>
+    <t>Kazakh</t>
+  </si>
+  <si>
+    <t>Kikuyu</t>
+  </si>
+  <si>
+    <t>Kinyarwanda</t>
+  </si>
+  <si>
+    <t>Kirghiz</t>
+  </si>
+  <si>
+    <t>Komi</t>
+  </si>
+  <si>
+    <t>Kongo</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Kuanyama</t>
+  </si>
+  <si>
+    <t>Kurdish</t>
+  </si>
+  <si>
+    <t>Lao</t>
+  </si>
+  <si>
+    <t>Latin</t>
+  </si>
+  <si>
+    <t>Latvian</t>
+  </si>
+  <si>
+    <t>Limburgan</t>
+  </si>
+  <si>
+    <t>Lingala</t>
+  </si>
+  <si>
+    <t>Lithuanian</t>
+  </si>
+  <si>
+    <t>L-PUNJABI</t>
+  </si>
+  <si>
+    <t>Luba-Katanga</t>
+  </si>
+  <si>
+    <t>Luxembourgish</t>
+  </si>
+  <si>
+    <t>Macedonian</t>
+  </si>
+  <si>
+    <t>Malagasy</t>
+  </si>
+  <si>
+    <t>Malayalam</t>
+  </si>
+  <si>
+    <t>Maltese</t>
+  </si>
+  <si>
+    <t>Manx</t>
+  </si>
+  <si>
+    <t>Maori</t>
+  </si>
+  <si>
+    <t>Marathi</t>
+  </si>
+  <si>
+    <t>Marshallese</t>
+  </si>
+  <si>
+    <t>Mongolian</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Navajo</t>
+  </si>
+  <si>
+    <t>Ndonga</t>
+  </si>
+  <si>
+    <t>Nepali</t>
+  </si>
+  <si>
+    <t>Northern Sami</t>
+  </si>
+  <si>
+    <t>North Ndebele</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>Norwegian Bokmål</t>
+  </si>
+  <si>
+    <t>Norwegian Nynorsk</t>
+  </si>
+  <si>
+    <t>Nzima</t>
+  </si>
+  <si>
+    <t>Occitan</t>
+  </si>
+  <si>
+    <t>Ojibwa</t>
+  </si>
+  <si>
+    <t>Oriya</t>
+  </si>
+  <si>
+    <t>Oromo</t>
+  </si>
+  <si>
+    <t>Ossetian</t>
+  </si>
+  <si>
+    <t>Pali</t>
+  </si>
+  <si>
+    <t>Panjabi</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>Pushto</t>
+  </si>
+  <si>
+    <t>Quechua</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>Romansh</t>
+  </si>
+  <si>
+    <t>Romany</t>
+  </si>
+  <si>
+    <t>Rundi</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Samoan</t>
+  </si>
+  <si>
+    <t>Sango</t>
+  </si>
+  <si>
+    <t>Sanskrit</t>
+  </si>
+  <si>
+    <t>Sardinian</t>
+  </si>
+  <si>
+    <t>Serbian</t>
+  </si>
+  <si>
+    <t>Shona</t>
+  </si>
+  <si>
+    <t>Sichuan Yi</t>
+  </si>
+  <si>
+    <t>Sindhi</t>
+  </si>
+  <si>
+    <t>Sinhala</t>
+  </si>
+  <si>
+    <t>Slovak</t>
+  </si>
+  <si>
+    <t>Slovenian</t>
+  </si>
+  <si>
+    <t>Somali</t>
+  </si>
+  <si>
+    <t>Sotho</t>
+  </si>
+  <si>
+    <t>South Ndebele</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Sundanese</t>
+  </si>
+  <si>
+    <t>Swahili</t>
+  </si>
+  <si>
+    <t>Swati</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>Tagalog</t>
+  </si>
+  <si>
+    <t>Tahitian</t>
+  </si>
+  <si>
+    <t>Tajik</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Tatar</t>
+  </si>
+  <si>
+    <t>Telugu</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>Tibetan</t>
+  </si>
+  <si>
+    <t>Tigrinya</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Tsonga</t>
+  </si>
+  <si>
+    <t>Tswana</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>Turkmen</t>
+  </si>
+  <si>
+    <t>Twi</t>
+  </si>
+  <si>
+    <t>Uighur</t>
+  </si>
+  <si>
+    <t>Ukranian</t>
+  </si>
+  <si>
+    <t>Urdu</t>
+  </si>
+  <si>
+    <t>Uzbek</t>
+  </si>
+  <si>
+    <t>Venda</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>Volapük</t>
+  </si>
+  <si>
+    <t>Walloon</t>
+  </si>
+  <si>
+    <t>Welsh</t>
+  </si>
+  <si>
+    <t>Western Frisian</t>
+  </si>
+  <si>
+    <t>Wolof</t>
+  </si>
+  <si>
+    <t>Xhosa</t>
+  </si>
+  <si>
+    <t>Yiddish</t>
+  </si>
+  <si>
+    <t>Yoruba</t>
+  </si>
+  <si>
+    <t>Zhuang</t>
+  </si>
+  <si>
+    <t>Zulu</t>
+  </si>
+  <si>
+    <t>Jahid</t>
   </si>
 </sst>
 </file>
@@ -415,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -538,12 +1102,953 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D187"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="H162" sqref="H162"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>203</v>
+      </c>
+      <c r="D176" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>